<commit_message>
£MHC FY22 presentation notes
</commit_message>
<xml_diff>
--- a/Overview - Space.xlsx
+++ b/Overview - Space.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20395"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20396"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E44ABC4-5EE4-45E2-9ECB-2D0B3BBFFDEA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC7979A9-7B8B-4DA2-972E-4B2588B95A3E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{AAD1FAE1-6B90-4A6C-91C2-DBC83F1146F1}"/>
   </bookViews>
@@ -235,7 +235,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -254,10 +254,13 @@
     <xf numFmtId="17" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -292,7 +295,7 @@
         </row>
         <row r="6">
           <cell r="C6">
-            <v>1.66</v>
+            <v>0.34</v>
           </cell>
         </row>
         <row r="7">
@@ -302,7 +305,7 @@
         </row>
         <row r="8">
           <cell r="C8">
-            <v>556.79079073999992</v>
+            <v>114.04148726</v>
           </cell>
         </row>
         <row r="11">
@@ -312,7 +315,7 @@
         </row>
         <row r="12">
           <cell r="C12">
-            <v>534.06979073999992</v>
+            <v>91.320487259999993</v>
           </cell>
         </row>
         <row r="28">
@@ -682,7 +685,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="N9" sqref="N9"/>
+      <selection pane="bottomRight" activeCell="F2" sqref="F2:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -708,7 +711,7 @@
       <c r="E2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="11" t="s">
         <v>11</v>
       </c>
       <c r="G2" s="3" t="s">
@@ -746,15 +749,15 @@
       <c r="E3" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="10">
-        <v>4.5149999999999997</v>
+      <c r="F3" s="12">
+        <v>4.04</v>
       </c>
       <c r="G3" s="7">
         <v>473.26</v>
       </c>
       <c r="H3" s="7">
         <f>F3*G3</f>
-        <v>2136.7689</v>
+        <v>1911.9703999999999</v>
       </c>
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
@@ -775,15 +778,15 @@
       <c r="E4" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="10">
-        <v>4.2519999999999998</v>
+      <c r="F4" s="12">
+        <v>4.05</v>
       </c>
       <c r="G4" s="7">
         <v>274.56</v>
       </c>
       <c r="H4" s="7">
         <f>F4*G4</f>
-        <v>1167.42912</v>
+        <v>1111.9679999999998</v>
       </c>
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
@@ -805,9 +808,9 @@
       <c r="E5" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="12">
         <f>[1]Main!$C$6</f>
-        <v>1.66</v>
+        <v>0.34</v>
       </c>
       <c r="G5" s="7">
         <f>[1]Main!$C$7</f>
@@ -815,7 +818,7 @@
       </c>
       <c r="H5" s="8">
         <f>[1]Main!$C$8</f>
-        <v>556.79079073999992</v>
+        <v>114.04148726</v>
       </c>
       <c r="I5" s="8">
         <f>[1]Main!$C$11</f>
@@ -823,7 +826,7 @@
       </c>
       <c r="J5" s="8">
         <f>[1]Main!$C$12</f>
-        <v>534.06979073999992</v>
+        <v>91.320487259999993</v>
       </c>
       <c r="K5" s="9" t="str">
         <f>[1]Main!$C$28</f>
@@ -850,15 +853,15 @@
       <c r="E6" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="1">
-        <v>0.51</v>
+      <c r="F6" s="12">
+        <v>0.42499999999999999</v>
       </c>
       <c r="G6" s="7">
         <v>211.93</v>
       </c>
       <c r="H6" s="7">
         <f>F6*G6</f>
-        <v>108.0843</v>
+        <v>90.070250000000001</v>
       </c>
       <c r="I6" s="7"/>
       <c r="K6" s="5"/>
@@ -880,15 +883,15 @@
       <c r="E7" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="10">
-        <v>0.92669999999999997</v>
+      <c r="F7" s="12">
+        <v>0.58499999999999996</v>
       </c>
       <c r="G7" s="7">
         <v>84.15</v>
       </c>
       <c r="H7" s="7">
         <f>F7*G7</f>
-        <v>77.981805000000008</v>
+        <v>49.22775</v>
       </c>
       <c r="I7" s="7"/>
       <c r="K7" s="5"/>
@@ -900,6 +903,7 @@
     <row r="8" spans="2:14" x14ac:dyDescent="0.2">
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
+      <c r="F8" s="12"/>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
@@ -919,9 +923,8 @@
       <c r="E9" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="1">
-        <f>[2]Main!$C$6</f>
-        <v>3.95</v>
+      <c r="F9" s="12">
+        <v>3.03</v>
       </c>
       <c r="G9" s="7">
         <f>[2]Main!$C$7</f>
@@ -1016,7 +1019,7 @@
       <c r="H13" s="1">
         <v>20.43</v>
       </c>
-      <c r="I13" s="11" t="s">
+      <c r="I13" s="10" t="s">
         <v>36</v>
       </c>
       <c r="K13" s="5"/>
@@ -1044,7 +1047,7 @@
       <c r="H14" s="1">
         <v>13.08</v>
       </c>
-      <c r="I14" s="11" t="s">
+      <c r="I14" s="10" t="s">
         <v>36</v>
       </c>
       <c r="K14" s="5"/>

</xml_diff>